<commit_message>
Add support for foreign-exchange rates
</commit_message>
<xml_diff>
--- a/PMStockQuote/PMStockQuote.xlsx
+++ b/PMStockQuote/PMStockQuote.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PMStockQuote\Source\PMStockQuote\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PMStockQuote\Source-Codeplex\pmstockquote\PMStockQuote\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>MSFT</t>
   </si>
@@ -45,14 +45,34 @@
   </si>
   <si>
     <t>GOOG</t>
+  </si>
+  <si>
+    <t>USDEUR</t>
+  </si>
+  <si>
+    <t>Stock Quotes</t>
+  </si>
+  <si>
+    <t>FX Rates</t>
+  </si>
+  <si>
+    <t>EURUSD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -80,11 +100,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -103,9 +124,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -143,7 +164,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -215,7 +236,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -365,77 +386,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="A1" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="str">
-        <f>_xll.PSQ(A2,"NAME")</f>
-        <v>Microsoft Corpora</v>
-      </c>
-      <c r="C2">
-        <f>_xll.PSQ(A2)</f>
-        <v>28.045000000000002</v>
-      </c>
-      <c r="D2" t="str">
-        <f>_xll.PSQ(A2,"DATE")</f>
-        <v>19.02.2013</v>
-      </c>
-      <c r="E2" t="str">
-        <f>_xll.PSQ(A2,"TIME")</f>
-        <v>16:00</v>
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B3" t="str">
         <f>_xll.PSQ(A3,"NAME")</f>
-        <v>Google Inc.</v>
+        <v>Microsoft Corpora</v>
       </c>
       <c r="C3">
         <f>_xll.PSQ(A3)</f>
-        <v>806.85</v>
+        <v>46.09</v>
       </c>
       <c r="D3" t="str">
         <f>_xll.PSQ(A3,"DATE")</f>
-        <v>19.02.2013</v>
+        <v>06.10.2014</v>
       </c>
       <c r="E3" t="str">
         <f>_xll.PSQ(A3,"TIME")</f>
-        <v>15:59</v>
+        <v>16:15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="str">
+        <f>_xll.PSQ(A4,"NAME")</f>
+        <v>Google Inc.</v>
+      </c>
+      <c r="C4">
+        <f>_xll.PSQ(A4)</f>
+        <v>577.35</v>
+      </c>
+      <c r="D4" t="str">
+        <f>_xll.PSQ(A4,"DATE")</f>
+        <v>06.10.2014</v>
+      </c>
+      <c r="E4" t="str">
+        <f>_xll.PSQ(A4,"TIME")</f>
+        <v>16:00</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="str">
+        <f>_xll.PFX(A7,"NAME")</f>
+        <v>USD to EUR</v>
+      </c>
+      <c r="C7">
+        <f>_xll.PFX(A7)</f>
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="D7" t="str">
+        <f>_xll.PFX(A7,"DATE")</f>
+        <v>07.10.2014</v>
+      </c>
+      <c r="E7" t="str">
+        <f>_xll.PFX(A7,"TIME")</f>
+        <v>07:43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="str">
+        <f>_xll.PFX(A8,"NAME")</f>
+        <v>EUR to USD</v>
+      </c>
+      <c r="C8">
+        <f>_xll.PFX(A8)</f>
+        <v>1.2595000000000001</v>
+      </c>
+      <c r="D8" t="str">
+        <f>_xll.PFX(A8,"DATE")</f>
+        <v>07.10.2014</v>
+      </c>
+      <c r="E8" t="str">
+        <f>_xll.PFX(A8,"TIME")</f>
+        <v>07:43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Replaced Yahoo Finance API by Google Finance API
Yahoo Finance got terminated by Yahoo on 11/01/2017.
</commit_message>
<xml_diff>
--- a/PMStockQuote/PMStockQuote.xlsx
+++ b/PMStockQuote/PMStockQuote.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PMStockQuote\Source-Codeplex\pmstockquote\PMStockQuote\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbaurle\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21990" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,45 +24,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
-  <si>
-    <t>MSFT</t>
-  </si>
-  <si>
-    <t>Symbol</t>
-  </si>
-  <si>
-    <t>Quote</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>GOOG</t>
-  </si>
-  <si>
-    <t>USDEUR</t>
-  </si>
-  <si>
-    <t>Stock Quotes</t>
-  </si>
-  <si>
-    <t>FX Rates</t>
-  </si>
-  <si>
-    <t>EURUSD</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>LAST</t>
+  </si>
+  <si>
+    <t>OPEN</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>LOW52</t>
+  </si>
+  <si>
+    <t>HIGH52</t>
+  </si>
+  <si>
+    <t>VOLUME</t>
+  </si>
+  <si>
+    <t>CHANGE</t>
+  </si>
+  <si>
+    <t>CHANGEPERCENTAGE</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>TIME</t>
+  </si>
+  <si>
+    <t>TICKER</t>
+  </si>
+  <si>
+    <t>EXCHANGE</t>
+  </si>
+  <si>
+    <t>NSDAQ:GOOGL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -72,7 +87,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -97,18 +111,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Währung" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -124,7 +141,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -140,7 +157,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -152,7 +169,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -169,9 +186,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -199,14 +216,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -234,6 +268,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -386,144 +437,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="B2:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2">
+        <f>_xll.PSQ(B2)</f>
+        <v>1053.4000000000001</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <f>_xll.PSQ($B$2,E2)</f>
+        <v>1053.4000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F3" s="2">
+        <f>_xll.PSQ($B$2,E3)</f>
+        <v>1055.49</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="F4" s="2">
+        <f>_xll.PSQ($B$2,E4)</f>
+        <v>1052.7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="str">
-        <f>_xll.PSQ(A3,"NAME")</f>
-        <v>Microsoft Corpora</v>
-      </c>
-      <c r="C3">
-        <f>_xll.PSQ(A3)</f>
-        <v>46.09</v>
-      </c>
-      <c r="D3" t="str">
-        <f>_xll.PSQ(A3,"DATE")</f>
-        <v>06.10.2014</v>
-      </c>
-      <c r="E3" t="str">
-        <f>_xll.PSQ(A3,"TIME")</f>
-        <v>16:15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="str">
-        <f>_xll.PSQ(A4,"NAME")</f>
-        <v>Google Inc.</v>
-      </c>
-      <c r="C4">
-        <f>_xll.PSQ(A4)</f>
-        <v>577.35</v>
-      </c>
-      <c r="D4" t="str">
-        <f>_xll.PSQ(A4,"DATE")</f>
-        <v>06.10.2014</v>
-      </c>
-      <c r="E4" t="str">
-        <f>_xll.PSQ(A4,"TIME")</f>
-        <v>16:00</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
+      <c r="F5" s="2">
+        <f>_xll.PSQ($B$2,E5)</f>
+        <v>1058.05</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="F6" s="2">
+        <f>_xll.PSQ($B$2,E6)</f>
+        <v>789.62</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2">
+        <f>_xll.PSQ($B$2,E7)</f>
+        <v>1086.49</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2">
+        <f>_xll.PSQ($B$2,E8)</f>
+        <v>351</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="str">
-        <f>_xll.PFX(A7,"NAME")</f>
-        <v>USD to EUR</v>
-      </c>
-      <c r="C7">
-        <f>_xll.PFX(A7)</f>
-        <v>0.79400000000000004</v>
-      </c>
-      <c r="D7" t="str">
-        <f>_xll.PFX(A7,"DATE")</f>
-        <v>07.10.2014</v>
-      </c>
-      <c r="E7" t="str">
-        <f>_xll.PFX(A7,"TIME")</f>
-        <v>07:43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="F9" s="2">
+        <f>_xll.PSQ($B$2,E9)</f>
+        <v>-2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="2">
+        <f>_xll.PSQ($B$2,E10)</f>
+        <v>-0.24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="3" t="str">
+        <f>_xll.PSQ($B$2,E11)</f>
+        <v>Alphabet Inc</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="str">
-        <f>_xll.PFX(A8,"NAME")</f>
-        <v>EUR to USD</v>
-      </c>
-      <c r="C8">
-        <f>_xll.PFX(A8)</f>
-        <v>1.2595000000000001</v>
-      </c>
-      <c r="D8" t="str">
-        <f>_xll.PFX(A8,"DATE")</f>
-        <v>07.10.2014</v>
-      </c>
-      <c r="E8" t="str">
-        <f>_xll.PFX(A8,"TIME")</f>
-        <v>07:43</v>
+      <c r="F12" s="3" t="str">
+        <f>_xll.PSQ($B$2,E12)</f>
+        <v>02.01.2018</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="3" t="str">
+        <f>_xll.PSQ($B$2,E13)</f>
+        <v>11:18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="3" t="str">
+        <f>_xll.PSQ($B$2,E14)</f>
+        <v>GOOGL</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="3" t="str">
+        <f>_xll.PSQ($B$2,E15)</f>
+        <v>NASDAQ</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Added JSON.NET parser to parse JSON data more flexible - Added Ticker Data dialog to see JSON data - Added JSON reference and path logic to address all available information
</commit_message>
<xml_diff>
--- a/PMStockQuote/PMStockQuote.xlsx
+++ b/PMStockQuote/PMStockQuote.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbaurle\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\PMStockQuote\PMStockQuote\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>LAST</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>NSDAQ:GOOGL</t>
+  </si>
+  <si>
+    <t>financials/0/f_figures/0/annual</t>
+  </si>
+  <si>
+    <t>!financials/0/f_figures/0/annual</t>
   </si>
 </sst>
 </file>
@@ -78,7 +84,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +98,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,11 +127,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -437,154 +453,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F15"/>
+  <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="2">
         <f>_xll.PSQ(B2)</f>
-        <v>1053.4000000000001</v>
+        <v>1110.29</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2">
         <f>_xll.PSQ($B$2,E2)</f>
-        <v>1053.4000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E3" t="s">
+        <v>1110.29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="2">
         <f>_xll.PSQ($B$2,E3)</f>
-        <v>1055.49</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
+        <v>1103.45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="2">
         <f>_xll.PSQ($B$2,E4)</f>
-        <v>1052.7</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
+        <v>1101.8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="2">
         <f>_xll.PSQ($B$2,E5)</f>
-        <v>1058.05</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
+        <v>1113.58</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2">
         <f>_xll.PSQ($B$2,E6)</f>
-        <v>789.62</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
+        <v>811.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2">
         <f>_xll.PSQ($B$2,E7)</f>
-        <v>1086.49</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
+        <v>1113.58</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="4" t="str">
         <f>_xll.PSQ($B$2,E8)</f>
-        <v>351</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
+        <v>1.51M</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2">
         <f>_xll.PSQ($B$2,E9)</f>
-        <v>-2.5499999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
+        <v>14.53</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
         <f>_xll.PSQ($B$2,E10)</f>
-        <v>-0.24</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="3" t="str">
+      <c r="F11" s="5" t="str">
         <f>_xll.PSQ($B$2,E11)</f>
         <v>Alphabet Inc</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="3" t="str">
+      <c r="F12" s="5" t="str">
         <f>_xll.PSQ($B$2,E12)</f>
-        <v>02.01.2018</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
+        <v>07.01.2018</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="3" t="str">
+      <c r="F13" s="5" t="str">
         <f>_xll.PSQ($B$2,E13)</f>
-        <v>11:18</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
+        <v>20:20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="3" t="str">
+      <c r="F14" s="5" t="str">
         <f>_xll.PSQ($B$2,E14)</f>
         <v>GOOGL</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="3" t="str">
+      <c r="F15" s="5" t="str">
         <f>_xll.PSQ($B$2,E15)</f>
         <v>NASDAQ</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="4" t="str">
+        <f>_xll.PSQ($B$2,E17)</f>
+        <v>90,272.00</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="2">
+        <f>_xll.PSQ($B$2,E18)</f>
+        <v>90272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>